<commit_message>
Notule meeting 7, logbook Youssef and "planning"
+ notule meeting 7
+- logbook Youssef
+- "planning"
</commit_message>
<xml_diff>
--- a/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_youssef.xlsx
+++ b/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_youssef.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
   <si>
     <t>Dag:</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>Maandag: Vergadering gehouden over wat er te doen valt en informatie vragen voor een aantal documenten.</t>
+  </si>
+  <si>
+    <t>Dinsdag: Norule vergadering 7 gemaakt, planning bijgewerkt en begonnen met de pwp presentatie.</t>
   </si>
 </sst>
 </file>
@@ -1146,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="S86" sqref="S86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,8 +1401,12 @@
       <c r="H11" s="16">
         <v>3</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="I11" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
@@ -1408,7 +1415,9 @@
       <c r="D12" s="16">
         <v>3</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="16">
+        <v>3</v>
+      </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
@@ -1473,7 +1482,7 @@
       <c r="D16" s="37"/>
       <c r="E16" s="19">
         <f>SUM((D5,D6,D7,D8,D9,D10,D11,D12,E5,E6,E7,E8,E9,E10,E11,E12,F5,F6,F7,F8,F9,F10,F11,F12,G5,G6,G7,G8,G9,G10,G11,G12,H5,H6,H7,H8,H9,H10,H11,H12,I5,I6,I7,I8,I9,I10,I11,I12,J5,J6,J7,J8,J9,J10,J11,J12,D13,D14,E13,E14,F13,F14,G13,G14,H13,H14,I13,I14,J13,J14))</f>
-        <v>145.5</v>
+        <v>148.5</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -2354,8 +2363,8 @@
       <c r="J83" s="41"/>
     </row>
     <row r="84" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C84" s="31" t="s">
-        <v>24</v>
+      <c r="C84" s="25" t="s">
+        <v>89</v>
       </c>
       <c r="D84" s="26"/>
       <c r="E84" s="26"/>

</xml_diff>

<commit_message>
Updated logbook and audio meeting 8
+- logbook
+ audio meeting 8
</commit_message>
<xml_diff>
--- a/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_youssef.xlsx
+++ b/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_youssef.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
   <si>
     <t>Dag:</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Dinsdag: Norule vergadering 7 gemaakt, planning bijgewerkt en begonnen met de pwp presentatie.</t>
+  </si>
+  <si>
+    <t>Donderdag: Met Lukasz gepraat hoe we de presentatie gaan aanpakken en vergadering gehouden.</t>
   </si>
 </sst>
 </file>
@@ -1150,7 +1153,7 @@
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L72" sqref="L72"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,8 +1421,12 @@
       <c r="E12" s="16">
         <v>3</v>
       </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="16">
+        <v>3</v>
+      </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
@@ -1482,7 +1489,7 @@
       <c r="D16" s="37"/>
       <c r="E16" s="19">
         <f>SUM((D5,D6,D7,D8,D9,D10,D11,D12,E5,E6,E7,E8,E9,E10,E11,E12,F5,F6,F7,F8,F9,F10,F11,F12,G5,G6,G7,G8,G9,G10,G11,G12,H5,H6,H7,H8,H9,H10,H11,H12,I5,I6,I7,I8,I9,I10,I11,I12,J5,J6,J7,J8,J9,J10,J11,J12,D13,D14,E13,E14,F13,F14,G13,G14,H13,H14,I13,I14,J13,J14))</f>
-        <v>148.5</v>
+        <v>151.5</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -2387,8 +2394,8 @@
       <c r="J85" s="27"/>
     </row>
     <row r="86" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C86" s="32" t="s">
-        <v>26</v>
+      <c r="C86" s="28" t="s">
+        <v>90</v>
       </c>
       <c r="D86" s="29"/>
       <c r="E86" s="29"/>

</xml_diff>

<commit_message>
Updated Logbook, Last notule meeting 8
+- Logbook
+ Notule meeting 8
</commit_message>
<xml_diff>
--- a/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_youssef.xlsx
+++ b/Documentation/Documentation_made/logboeken/urenlijst_met_logboek_youssef.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
   <si>
     <t>Dag:</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Donderdag:</t>
   </si>
   <si>
-    <t>Vrijdag:</t>
-  </si>
-  <si>
     <t>Zaterdag:</t>
   </si>
   <si>
@@ -292,6 +289,9 @@
   </si>
   <si>
     <t>Donderdag: Met Lukasz gepraat hoe we de presentatie gaan aanpakken en vergadering gehouden.</t>
+  </si>
+  <si>
+    <t>Vrijdag: Notule laatste vergadering gemaakt, voorbereiding opleveren en laatset documenten updaten.</t>
   </si>
 </sst>
 </file>
@@ -772,15 +772,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -790,19 +838,22 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -812,57 +863,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1153,17 +1153,17 @@
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="38"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="17" t="s">
@@ -1208,7 +1208,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="16">
         <v>3</v>
@@ -1222,11 +1222,11 @@
       <c r="J5" s="16">
         <v>4</v>
       </c>
-      <c r="O5" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="46"/>
+      <c r="O5" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="49"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
@@ -1248,17 +1248,17 @@
         <v>3</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" s="6"/>
-      <c r="O6" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="52"/>
+      <c r="O6" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="27"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
@@ -1271,7 +1271,7 @@
         <v>5</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="16">
         <v>4.5</v>
@@ -1280,16 +1280,16 @@
         <v>3</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="O7" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="49"/>
+        <v>39</v>
+      </c>
+      <c r="O7" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="36"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
@@ -1302,7 +1302,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="16">
         <v>1</v>
@@ -1311,16 +1311,16 @@
         <v>3</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="O8" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="49"/>
+        <v>39</v>
+      </c>
+      <c r="O8" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="36"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
@@ -1333,7 +1333,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="16">
         <v>3</v>
@@ -1342,17 +1342,17 @@
         <v>3</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K9" s="6"/>
-      <c r="O9" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="49"/>
+      <c r="O9" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="36"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
@@ -1365,7 +1365,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="16">
         <v>5</v>
@@ -1374,16 +1374,16 @@
         <v>5</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="O10" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="55"/>
+      <c r="O10" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="33"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
@@ -1405,10 +1405,10 @@
         <v>3</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -1422,30 +1422,36 @@
         <v>3</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="16">
         <v>3</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
+      <c r="H12" s="16">
+        <v>3</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="16">
         <v>4</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" s="16">
         <v>6</v>
@@ -1454,7 +1460,7 @@
         <v>3</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1483,13 +1489,13 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="37"/>
+      <c r="D16" s="54"/>
       <c r="E16" s="19">
         <f>SUM((D5,D6,D7,D8,D9,D10,D11,D12,E5,E6,E7,E8,E9,E10,E11,E12,F5,F6,F7,F8,F9,F10,F11,F12,G5,G6,G7,G8,G9,G10,G11,G12,H5,H6,H7,H8,H9,H10,H11,H12,I5,I6,I7,I8,I9,I10,I11,I12,J5,J6,J7,J8,J9,J10,J11,J12,D13,D14,E13,E14,F13,F14,G13,G14,H13,H14,I13,I14,J13,J14))</f>
-        <v>151.5</v>
+        <v>154.5</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -1540,100 +1546,100 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="41"/>
+      <c r="C20" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
+      <c r="C21" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27"/>
+      <c r="C22" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="30"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="11"/>
-      <c r="C23" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="30"/>
+      <c r="C23" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="46"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="27"/>
+      <c r="C24" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="30"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
+      <c r="C25" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="30"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
-      <c r="C26" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="35"/>
+      <c r="C26" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="39"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
@@ -1664,100 +1670,100 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="41"/>
+      <c r="C29" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="42"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="27"/>
+      <c r="C30" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
-      <c r="C31" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="27"/>
+      <c r="C31" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
-      <c r="C32" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="30"/>
+      <c r="C32" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="46"/>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
-      <c r="C33" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="27"/>
+      <c r="C33" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="30"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
-      <c r="C34" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="27"/>
+      <c r="C34" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="30"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="10"/>
-      <c r="C35" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="35"/>
+      <c r="C35" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="39"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
@@ -1775,7 +1781,7 @@
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
@@ -1788,100 +1794,100 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="41"/>
+      <c r="C38" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="42"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="27"/>
+      <c r="C39" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="30"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
-      <c r="C40" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="27"/>
+      <c r="C40" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="30"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
-      <c r="C41" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="30"/>
+      <c r="C41" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="46"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
-      <c r="C42" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="27"/>
+      <c r="C42" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
-      <c r="C43" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="27"/>
+      <c r="C43" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
-      <c r="C44" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="35"/>
+      <c r="C44" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
@@ -1899,7 +1905,7 @@
       <c r="A46" s="6"/>
       <c r="B46" s="7"/>
       <c r="C46" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
@@ -1912,100 +1918,100 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="12"/>
-      <c r="C47" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="41"/>
+      <c r="C47" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="42"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
-      <c r="C48" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="27"/>
+      <c r="C48" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="30"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="27"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="30"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="30"/>
+      <c r="C50" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="46"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="27"/>
+      <c r="C51" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="30"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="27"/>
+      <c r="C52" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="30"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="35"/>
+      <c r="C53" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="39"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
@@ -2023,7 +2029,7 @@
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="20"/>
@@ -2036,92 +2042,92 @@
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="40"/>
-      <c r="J56" s="41"/>
+      <c r="C56" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="42"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="26"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="27"/>
+      <c r="C57" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
+      <c r="J57" s="30"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="31" t="s">
+      <c r="C58" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
-      <c r="I58" s="26"/>
-      <c r="J58" s="27"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="29"/>
+      <c r="J58" s="30"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C59" s="28" t="s">
+      <c r="C59" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" s="45"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="46"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C60" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
-      <c r="G59" s="29"/>
-      <c r="H59" s="29"/>
-      <c r="I59" s="29"/>
-      <c r="J59" s="30"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C60" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="26"/>
-      <c r="I60" s="26"/>
-      <c r="J60" s="27"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="30"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C61" s="31" t="s">
+      <c r="C61" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="30"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C62" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D61" s="26"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="27"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C62" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="34"/>
-      <c r="G62" s="34"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="34"/>
-      <c r="J62" s="35"/>
+      <c r="D62" s="38"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+      <c r="J62" s="39"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C63" s="22"/>
@@ -2135,7 +2141,7 @@
     </row>
     <row r="64" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C64" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D64" s="20"/>
       <c r="E64" s="20"/>
@@ -2146,88 +2152,88 @@
       <c r="J64" s="20"/>
     </row>
     <row r="65" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C65" s="42" t="s">
+      <c r="C65" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="41"/>
+      <c r="E65" s="41"/>
+      <c r="F65" s="41"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="41"/>
+      <c r="I65" s="41"/>
+      <c r="J65" s="42"/>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C66" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="D65" s="40"/>
-      <c r="E65" s="40"/>
-      <c r="F65" s="40"/>
-      <c r="G65" s="40"/>
-      <c r="H65" s="40"/>
-      <c r="I65" s="40"/>
-      <c r="J65" s="41"/>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C66" s="25" t="s">
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="30"/>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C67" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="D66" s="26"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="26"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="26"/>
-      <c r="I66" s="26"/>
-      <c r="J66" s="27"/>
-    </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C67" s="25" t="s">
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
+      <c r="G67" s="29"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="30"/>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C68" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="26"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="26"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="26"/>
-      <c r="I67" s="26"/>
-      <c r="J67" s="27"/>
-    </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C68" s="28" t="s">
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="45"/>
+      <c r="G68" s="45"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="45"/>
+      <c r="J68" s="46"/>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C69" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="30"/>
-    </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C69" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D69" s="26"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="26"/>
-      <c r="I69" s="26"/>
-      <c r="J69" s="27"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="30"/>
     </row>
     <row r="70" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C70" s="31" t="s">
+      <c r="C70" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="30"/>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C71" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D70" s="26"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="26"/>
-      <c r="G70" s="26"/>
-      <c r="H70" s="26"/>
-      <c r="I70" s="26"/>
-      <c r="J70" s="27"/>
-    </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C71" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D71" s="34"/>
-      <c r="E71" s="34"/>
-      <c r="F71" s="34"/>
-      <c r="G71" s="34"/>
-      <c r="H71" s="34"/>
-      <c r="I71" s="34"/>
-      <c r="J71" s="35"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="38"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="39"/>
     </row>
     <row r="72" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C72" s="22"/>
@@ -2241,7 +2247,7 @@
     </row>
     <row r="73" spans="3:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C73" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D73" s="20"/>
       <c r="E73" s="20"/>
@@ -2252,88 +2258,88 @@
       <c r="J73" s="20"/>
     </row>
     <row r="74" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C74" s="42" t="s">
+      <c r="C74" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D74" s="41"/>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="41"/>
+      <c r="I74" s="41"/>
+      <c r="J74" s="42"/>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C75" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="D74" s="40"/>
-      <c r="E74" s="40"/>
-      <c r="F74" s="40"/>
-      <c r="G74" s="40"/>
-      <c r="H74" s="40"/>
-      <c r="I74" s="40"/>
-      <c r="J74" s="41"/>
-    </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C75" s="25" t="s">
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="30"/>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C76" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="D75" s="26"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="26"/>
-      <c r="G75" s="26"/>
-      <c r="H75" s="26"/>
-      <c r="I75" s="26"/>
-      <c r="J75" s="27"/>
-    </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C76" s="25" t="s">
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="30"/>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C77" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D77" s="45"/>
+      <c r="E77" s="45"/>
+      <c r="F77" s="45"/>
+      <c r="G77" s="45"/>
+      <c r="H77" s="45"/>
+      <c r="I77" s="45"/>
+      <c r="J77" s="46"/>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C78" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="D76" s="26"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="26"/>
-      <c r="G76" s="26"/>
-      <c r="H76" s="26"/>
-      <c r="I76" s="26"/>
-      <c r="J76" s="27"/>
-    </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C77" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="D77" s="29"/>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="29"/>
-      <c r="I77" s="29"/>
-      <c r="J77" s="30"/>
-    </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C78" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D78" s="26"/>
-      <c r="E78" s="26"/>
-      <c r="F78" s="26"/>
-      <c r="G78" s="26"/>
-      <c r="H78" s="26"/>
-      <c r="I78" s="26"/>
-      <c r="J78" s="27"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
+      <c r="J78" s="30"/>
     </row>
     <row r="79" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C79" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D79" s="26"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="26"/>
-      <c r="G79" s="26"/>
-      <c r="H79" s="26"/>
-      <c r="I79" s="26"/>
-      <c r="J79" s="27"/>
+      <c r="C79" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="29"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="30"/>
     </row>
     <row r="80" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C80" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D80" s="34"/>
-      <c r="E80" s="34"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="34"/>
-      <c r="H80" s="34"/>
-      <c r="I80" s="34"/>
-      <c r="J80" s="35"/>
+      <c r="C80" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="38"/>
+      <c r="J80" s="39"/>
     </row>
     <row r="81" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C81" s="22"/>
@@ -2347,7 +2353,7 @@
     </row>
     <row r="82" spans="3:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C82" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D82" s="20"/>
       <c r="E82" s="20"/>
@@ -2358,88 +2364,88 @@
       <c r="J82" s="20"/>
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C83" s="42" t="s">
+      <c r="C83" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D83" s="41"/>
+      <c r="E83" s="41"/>
+      <c r="F83" s="41"/>
+      <c r="G83" s="41"/>
+      <c r="H83" s="41"/>
+      <c r="I83" s="41"/>
+      <c r="J83" s="42"/>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C84" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="D83" s="40"/>
-      <c r="E83" s="40"/>
-      <c r="F83" s="40"/>
-      <c r="G83" s="40"/>
-      <c r="H83" s="40"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="41"/>
-    </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C84" s="25" t="s">
+      <c r="D84" s="29"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="29"/>
+      <c r="H84" s="29"/>
+      <c r="I84" s="29"/>
+      <c r="J84" s="30"/>
+    </row>
+    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C85" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="30"/>
+    </row>
+    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C86" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="D84" s="26"/>
-      <c r="E84" s="26"/>
-      <c r="F84" s="26"/>
-      <c r="G84" s="26"/>
-      <c r="H84" s="26"/>
-      <c r="I84" s="26"/>
-      <c r="J84" s="27"/>
-    </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C85" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="D85" s="26"/>
-      <c r="E85" s="26"/>
-      <c r="F85" s="26"/>
-      <c r="G85" s="26"/>
-      <c r="H85" s="26"/>
-      <c r="I85" s="26"/>
-      <c r="J85" s="27"/>
-    </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C86" s="28" t="s">
+      <c r="D86" s="45"/>
+      <c r="E86" s="45"/>
+      <c r="F86" s="45"/>
+      <c r="G86" s="45"/>
+      <c r="H86" s="45"/>
+      <c r="I86" s="45"/>
+      <c r="J86" s="46"/>
+    </row>
+    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C87" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="D86" s="29"/>
-      <c r="E86" s="29"/>
-      <c r="F86" s="29"/>
-      <c r="G86" s="29"/>
-      <c r="H86" s="29"/>
-      <c r="I86" s="29"/>
-      <c r="J86" s="30"/>
-    </row>
-    <row r="87" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C87" s="31" t="s">
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="30"/>
+    </row>
+    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C88" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="26"/>
-      <c r="H87" s="26"/>
-      <c r="I87" s="26"/>
-      <c r="J87" s="27"/>
-    </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C88" s="31" t="s">
+      <c r="D88" s="29"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="29"/>
+      <c r="J88" s="30"/>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C89" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="26"/>
-      <c r="E88" s="26"/>
-      <c r="F88" s="26"/>
-      <c r="G88" s="26"/>
-      <c r="H88" s="26"/>
-      <c r="I88" s="26"/>
-      <c r="J88" s="27"/>
-    </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C89" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D89" s="34"/>
-      <c r="E89" s="34"/>
-      <c r="F89" s="34"/>
-      <c r="G89" s="34"/>
-      <c r="H89" s="34"/>
-      <c r="I89" s="34"/>
-      <c r="J89" s="35"/>
+      <c r="D89" s="38"/>
+      <c r="E89" s="38"/>
+      <c r="F89" s="38"/>
+      <c r="G89" s="38"/>
+      <c r="H89" s="38"/>
+      <c r="I89" s="38"/>
+      <c r="J89" s="39"/>
     </row>
     <row r="90" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C90" s="22"/>
@@ -2453,7 +2459,7 @@
     </row>
     <row r="91" spans="3:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C91" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D91" s="20"/>
       <c r="E91" s="20"/>
@@ -2464,88 +2470,88 @@
       <c r="J91" s="20"/>
     </row>
     <row r="92" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C92" s="39" t="s">
+      <c r="C92" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="D92" s="40"/>
-      <c r="E92" s="40"/>
-      <c r="F92" s="40"/>
-      <c r="G92" s="40"/>
-      <c r="H92" s="40"/>
-      <c r="I92" s="40"/>
-      <c r="J92" s="41"/>
+      <c r="D92" s="41"/>
+      <c r="E92" s="41"/>
+      <c r="F92" s="41"/>
+      <c r="G92" s="41"/>
+      <c r="H92" s="41"/>
+      <c r="I92" s="41"/>
+      <c r="J92" s="42"/>
     </row>
     <row r="93" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C93" s="31" t="s">
+      <c r="C93" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D93" s="26"/>
-      <c r="E93" s="26"/>
-      <c r="F93" s="26"/>
-      <c r="G93" s="26"/>
-      <c r="H93" s="26"/>
-      <c r="I93" s="26"/>
-      <c r="J93" s="27"/>
+      <c r="D93" s="29"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="29"/>
+      <c r="I93" s="29"/>
+      <c r="J93" s="30"/>
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C94" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D94" s="26"/>
-      <c r="E94" s="26"/>
-      <c r="F94" s="26"/>
-      <c r="G94" s="26"/>
-      <c r="H94" s="26"/>
-      <c r="I94" s="26"/>
-      <c r="J94" s="27"/>
+      <c r="C94" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="29"/>
+      <c r="J94" s="30"/>
     </row>
     <row r="95" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C95" s="32" t="s">
+      <c r="C95" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D95" s="29"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="29"/>
-      <c r="G95" s="29"/>
-      <c r="H95" s="29"/>
-      <c r="I95" s="29"/>
-      <c r="J95" s="30"/>
+      <c r="D95" s="45"/>
+      <c r="E95" s="45"/>
+      <c r="F95" s="45"/>
+      <c r="G95" s="45"/>
+      <c r="H95" s="45"/>
+      <c r="I95" s="45"/>
+      <c r="J95" s="46"/>
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C96" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D96" s="26"/>
-      <c r="E96" s="26"/>
-      <c r="F96" s="26"/>
-      <c r="G96" s="26"/>
-      <c r="H96" s="26"/>
-      <c r="I96" s="26"/>
-      <c r="J96" s="27"/>
+      <c r="C96" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="D96" s="29"/>
+      <c r="E96" s="29"/>
+      <c r="F96" s="29"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="30"/>
     </row>
     <row r="97" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C97" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D97" s="26"/>
-      <c r="E97" s="26"/>
-      <c r="F97" s="26"/>
-      <c r="G97" s="26"/>
-      <c r="H97" s="26"/>
-      <c r="I97" s="26"/>
-      <c r="J97" s="27"/>
+      <c r="C97" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="30"/>
     </row>
     <row r="98" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C98" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D98" s="34"/>
-      <c r="E98" s="34"/>
-      <c r="F98" s="34"/>
-      <c r="G98" s="34"/>
-      <c r="H98" s="34"/>
-      <c r="I98" s="34"/>
-      <c r="J98" s="35"/>
+      <c r="C98" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D98" s="38"/>
+      <c r="E98" s="38"/>
+      <c r="F98" s="38"/>
+      <c r="G98" s="38"/>
+      <c r="H98" s="38"/>
+      <c r="I98" s="38"/>
+      <c r="J98" s="39"/>
     </row>
     <row r="100" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C100" s="9"/>
@@ -2629,6 +2635,61 @@
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="C30:J30"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="C32:J32"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="C21:J21"/>
+    <mergeCell ref="C29:J29"/>
+    <mergeCell ref="C33:J33"/>
+    <mergeCell ref="C38:J38"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="C41:J41"/>
+    <mergeCell ref="C34:J34"/>
+    <mergeCell ref="C35:J35"/>
+    <mergeCell ref="C50:J50"/>
+    <mergeCell ref="C51:J51"/>
+    <mergeCell ref="C52:J52"/>
+    <mergeCell ref="C53:J53"/>
+    <mergeCell ref="C42:J42"/>
+    <mergeCell ref="C43:J43"/>
+    <mergeCell ref="C44:J44"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="C80:J80"/>
+    <mergeCell ref="C98:J98"/>
+    <mergeCell ref="C88:J88"/>
+    <mergeCell ref="C89:J89"/>
+    <mergeCell ref="C92:J92"/>
+    <mergeCell ref="C93:J93"/>
+    <mergeCell ref="C94:J94"/>
+    <mergeCell ref="C96:J96"/>
+    <mergeCell ref="C97:J97"/>
+    <mergeCell ref="C95:J95"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="O7:Q7"/>
+    <mergeCell ref="C69:J69"/>
+    <mergeCell ref="C61:J61"/>
+    <mergeCell ref="C70:J70"/>
+    <mergeCell ref="C62:J62"/>
+    <mergeCell ref="C65:J65"/>
+    <mergeCell ref="C66:J66"/>
+    <mergeCell ref="C67:J67"/>
+    <mergeCell ref="C68:J68"/>
+    <mergeCell ref="C56:J56"/>
+    <mergeCell ref="C57:J57"/>
+    <mergeCell ref="C58:J58"/>
+    <mergeCell ref="C59:J59"/>
+    <mergeCell ref="C60:J60"/>
+    <mergeCell ref="C49:J49"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="C87:J87"/>
     <mergeCell ref="O10:Q10"/>
@@ -2645,61 +2706,6 @@
     <mergeCell ref="C77:J77"/>
     <mergeCell ref="C78:J78"/>
     <mergeCell ref="C79:J79"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="O7:Q7"/>
-    <mergeCell ref="C69:J69"/>
-    <mergeCell ref="C61:J61"/>
-    <mergeCell ref="C70:J70"/>
-    <mergeCell ref="C62:J62"/>
-    <mergeCell ref="C65:J65"/>
-    <mergeCell ref="C66:J66"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="C68:J68"/>
-    <mergeCell ref="C56:J56"/>
-    <mergeCell ref="C57:J57"/>
-    <mergeCell ref="C58:J58"/>
-    <mergeCell ref="C59:J59"/>
-    <mergeCell ref="C60:J60"/>
-    <mergeCell ref="C49:J49"/>
-    <mergeCell ref="C80:J80"/>
-    <mergeCell ref="C98:J98"/>
-    <mergeCell ref="C88:J88"/>
-    <mergeCell ref="C89:J89"/>
-    <mergeCell ref="C92:J92"/>
-    <mergeCell ref="C93:J93"/>
-    <mergeCell ref="C94:J94"/>
-    <mergeCell ref="C96:J96"/>
-    <mergeCell ref="C97:J97"/>
-    <mergeCell ref="C95:J95"/>
-    <mergeCell ref="C50:J50"/>
-    <mergeCell ref="C51:J51"/>
-    <mergeCell ref="C52:J52"/>
-    <mergeCell ref="C53:J53"/>
-    <mergeCell ref="C42:J42"/>
-    <mergeCell ref="C43:J43"/>
-    <mergeCell ref="C44:J44"/>
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C48:J48"/>
-    <mergeCell ref="C33:J33"/>
-    <mergeCell ref="C38:J38"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="C40:J40"/>
-    <mergeCell ref="C41:J41"/>
-    <mergeCell ref="C34:J34"/>
-    <mergeCell ref="C35:J35"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="C21:J21"/>
-    <mergeCell ref="C29:J29"/>
-    <mergeCell ref="C30:J30"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="C32:J32"/>
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>